<commit_message>
CO hard wired cpu
</commit_message>
<xml_diff>
--- a/computer organization/输出信号表.xlsx
+++ b/computer organization/输出信号表.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git-repos\HomeWork\computer organization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D81FF6-78A4-47B6-9902-B927FA4512D0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF9D9669-306F-4798-BBB4-8590EEBB7FB3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16860" windowHeight="6945" xr2:uid="{6005AAD0-0933-48B5-8F40-74FA52248108}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16860" windowHeight="6945" activeTab="1" xr2:uid="{6005AAD0-0933-48B5-8F40-74FA52248108}"/>
   </bookViews>
   <sheets>
     <sheet name="输出信号一览" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="83">
   <si>
     <t>SBUS</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -68,10 +68,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>SST0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>SHORT</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -264,22 +260,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>W1&amp;ST0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>W2&amp;ST0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>W2&amp;ST1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>W1&amp;ST1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>SWD011读寄存器</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -300,15 +280,76 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ST1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>W1(1)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>W2+W3(1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SWD000取指执行</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>!ST</t>
+  </si>
+  <si>
+    <t>SST</t>
+  </si>
+  <si>
+    <t>W2&amp;!ST</t>
+  </si>
+  <si>
+    <t>ST</t>
+  </si>
+  <si>
+    <t>W1&amp;!ST</t>
+  </si>
+  <si>
+    <t>W1&amp;ST</t>
+  </si>
+  <si>
+    <t>W2&amp;ST</t>
+  </si>
+  <si>
+    <t>OUT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>W2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>!ST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>右侧为扩展指令</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>S[1110]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>W2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>XOR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NOT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>S[0101]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -675,7 +716,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60C2AF42-F6FC-4515-A33E-E3BD7A26C16F}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E2:E7"/>
     </sheetView>
   </sheetViews>
@@ -691,53 +732,53 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
         <v>26</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>27</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>28</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>29</v>
-      </c>
-      <c r="F1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
         <v>2</v>
@@ -748,7 +789,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
@@ -762,10 +803,10 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E5" t="s">
         <v>4</v>
@@ -773,10 +814,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E6" t="s">
         <v>5</v>
@@ -784,10 +825,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E7" t="s">
         <v>7</v>
@@ -795,7 +836,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="D8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -807,458 +848,556 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0739107-5A32-44E2-8FB0-BA045DEC7AFE}">
-  <dimension ref="A1:O37"/>
+  <dimension ref="A1:U39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="P2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H7" sqref="H7"/>
+      <selection pane="bottomRight" activeCell="U24" sqref="U24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.33203125" customWidth="1"/>
+    <col min="13" max="16" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.33203125" customWidth="1"/>
+    <col min="18" max="18" width="14.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.4">
       <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
         <v>32</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>33</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>34</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>35</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>36</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>37</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>38</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>39</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
+        <v>73</v>
+      </c>
+      <c r="L1" t="s">
         <v>40</v>
       </c>
-      <c r="K1" t="s">
-        <v>41</v>
-      </c>
-      <c r="L1" t="s">
-        <v>52</v>
-      </c>
       <c r="M1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N1" t="s">
+        <v>51</v>
+      </c>
+      <c r="O1" t="s">
+        <v>58</v>
+      </c>
+      <c r="P1" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>60</v>
+      </c>
+      <c r="R1" t="s">
+        <v>76</v>
+      </c>
+      <c r="S1" t="s">
+        <v>77</v>
+      </c>
+      <c r="T1" t="s">
+        <v>80</v>
+      </c>
+      <c r="U1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" t="s">
+        <v>66</v>
+      </c>
+      <c r="P2" t="s">
         <v>63</v>
       </c>
-      <c r="N1" t="s">
-        <v>64</v>
-      </c>
-      <c r="O1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
+      <c r="Q2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
         <v>11</v>
       </c>
-      <c r="N2" t="s">
-        <v>69</v>
-      </c>
-      <c r="O2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
       <c r="F3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="L4" t="s">
-        <v>60</v>
+        <v>67</v>
+      </c>
+      <c r="M4" t="s">
+        <v>66</v>
       </c>
       <c r="N4" t="s">
-        <v>6</v>
-      </c>
-      <c r="O4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
+        <v>68</v>
+      </c>
+      <c r="P4" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="K5" t="s">
-        <v>42</v>
-      </c>
       <c r="L5" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
       <c r="M5" t="s">
         <v>66</v>
       </c>
       <c r="N5" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="O5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
+        <v>61</v>
+      </c>
+      <c r="P5" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" t="s">
+        <v>64</v>
+      </c>
+      <c r="J6" t="s">
+        <v>41</v>
+      </c>
+      <c r="K6" t="s">
+        <v>74</v>
+      </c>
+      <c r="S6" t="s">
+        <v>41</v>
+      </c>
+      <c r="T6" t="s">
+        <v>79</v>
+      </c>
+      <c r="U6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
         <v>19</v>
       </c>
-      <c r="B6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6" t="s">
-        <v>42</v>
-      </c>
-      <c r="D6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F6" t="s">
-        <v>42</v>
-      </c>
-      <c r="G6" t="s">
-        <v>70</v>
-      </c>
-      <c r="J6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" t="s">
+        <v>41</v>
+      </c>
+      <c r="S7" t="s">
+        <v>41</v>
+      </c>
+      <c r="T7" t="s">
+        <v>79</v>
+      </c>
+      <c r="U7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
         <v>20</v>
       </c>
-      <c r="B7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
         <v>21</v>
       </c>
-      <c r="B8" t="s">
-        <v>42</v>
-      </c>
-      <c r="C8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A9" t="s">
-        <v>22</v>
-      </c>
       <c r="D9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G9" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="J9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
+        <v>41</v>
+      </c>
+      <c r="K9" t="s">
+        <v>74</v>
+      </c>
+      <c r="S9" t="s">
+        <v>41</v>
+      </c>
+      <c r="T9" t="s">
+        <v>79</v>
+      </c>
+      <c r="U9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>0</v>
       </c>
-      <c r="L11" t="s">
+      <c r="M11" t="s">
+        <v>75</v>
+      </c>
+      <c r="N11" t="s">
+        <v>61</v>
+      </c>
+      <c r="P11" t="s">
         <v>66</v>
       </c>
-      <c r="N11" t="s">
-        <v>6</v>
-      </c>
-      <c r="O11" t="s">
+      <c r="Q11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" t="s">
+        <v>47</v>
+      </c>
+      <c r="P12" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="F12" t="s">
-        <v>48</v>
-      </c>
-      <c r="N12" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G13" t="s">
-        <v>48</v>
-      </c>
-      <c r="O13" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
+        <v>47</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>9</v>
       </c>
       <c r="F14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G14" t="s">
-        <v>42</v>
-      </c>
-      <c r="N14" t="s">
-        <v>6</v>
-      </c>
-      <c r="O14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
+        <v>41</v>
+      </c>
+      <c r="P14" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>14</v>
-      </c>
-      <c r="N16" t="s">
-        <v>68</v>
-      </c>
-      <c r="O16" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.4">
+        <v>13</v>
+      </c>
+      <c r="P16" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="H17" t="s">
+        <v>49</v>
+      </c>
+      <c r="I17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="A18" t="s">
         <v>24</v>
       </c>
-      <c r="H17" t="s">
-        <v>50</v>
-      </c>
-      <c r="I17" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A18" t="s">
-        <v>25</v>
-      </c>
       <c r="J18" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.4">
+        <v>41</v>
+      </c>
+      <c r="M18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>5</v>
       </c>
-      <c r="L23" t="s">
-        <v>66</v>
-      </c>
-      <c r="M23" t="s">
-        <v>66</v>
-      </c>
       <c r="N23" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="O23" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.4">
+        <v>61</v>
+      </c>
+      <c r="P23" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>7</v>
       </c>
       <c r="B24" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24" t="s">
+        <v>41</v>
+      </c>
+      <c r="E24" t="s">
+        <v>41</v>
+      </c>
+      <c r="F24" t="s">
+        <v>47</v>
+      </c>
+      <c r="N24" t="s">
+        <v>61</v>
+      </c>
+      <c r="S24" t="s">
+        <v>41</v>
+      </c>
+      <c r="T24" t="s">
+        <v>79</v>
+      </c>
+      <c r="U24" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="A25" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="A26" t="s">
         <v>42</v>
       </c>
-      <c r="C24" t="s">
-        <v>42</v>
-      </c>
-      <c r="D24" t="s">
-        <v>42</v>
-      </c>
-      <c r="E24" t="s">
-        <v>42</v>
-      </c>
-      <c r="F24" t="s">
+      <c r="B26" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="A27" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27" t="s">
+        <v>41</v>
+      </c>
+      <c r="T27" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="A28" t="s">
+        <v>44</v>
+      </c>
+      <c r="D28" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="A29" t="s">
+        <v>45</v>
+      </c>
+      <c r="E29" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="A30" t="s">
+        <v>46</v>
+      </c>
+      <c r="F30" t="s">
+        <v>41</v>
+      </c>
+      <c r="G30" t="s">
+        <v>47</v>
+      </c>
+      <c r="K30" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="A31" t="s">
         <v>48</v>
       </c>
-      <c r="L24" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A25" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A26" t="s">
-        <v>43</v>
-      </c>
-      <c r="B26" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A27" t="s">
-        <v>44</v>
-      </c>
-      <c r="C27" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A28" t="s">
-        <v>45</v>
-      </c>
-      <c r="D28" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A29" t="s">
-        <v>46</v>
-      </c>
-      <c r="E29" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A30" t="s">
-        <v>47</v>
-      </c>
-      <c r="F30" t="s">
-        <v>42</v>
-      </c>
-      <c r="G30" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A31" t="s">
-        <v>49</v>
-      </c>
       <c r="G31" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J31" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.4">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
+        <v>78</v>
+      </c>
+      <c r="S32" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="A33" t="s">
+        <v>82</v>
+      </c>
+      <c r="U33" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="A34" t="s">
+        <v>52</v>
+      </c>
+      <c r="N34" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="A35" t="s">
         <v>53</v>
       </c>
-      <c r="L32" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A33" t="s">
+      <c r="N35" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="A36" t="s">
         <v>54</v>
       </c>
-      <c r="L33" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A34" t="s">
+      <c r="N36" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="A37" t="s">
         <v>55</v>
       </c>
-      <c r="L34" t="s">
+      <c r="N37" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="A38" t="s">
+        <v>56</v>
+      </c>
+      <c r="O38" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A35" t="s">
-        <v>56</v>
-      </c>
-      <c r="L35" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A36" t="s">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="A39" t="s">
         <v>57</v>
       </c>
-      <c r="M36" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A37" t="s">
-        <v>58</v>
-      </c>
-      <c r="M37" t="s">
-        <v>42</v>
+      <c r="O39" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>